<commit_message>
fix: ajuste de bug no windows
</commit_message>
<xml_diff>
--- a/db/sod_database.xlsx
+++ b/db/sod_database.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sia</t>
+          <t>sia-estacio</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -475,12 +475,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>financ</t>
+          <t>financeiro</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Financeiro Estácio</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>novo_sistema</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Renomeado</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>novo_sistem</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Novo Sistema</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: ajuste na listagem dos usuários para ser exibido no novo padrão
</commit_message>
<xml_diff>
--- a/db/sod_database.xlsx
+++ b/db/sod_database.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,30 @@
       <c r="B6" t="inlineStr">
         <is>
           <t>Novo Sistema</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>teste2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Teste2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: Criada listagem e modal de criação e edição de Perfis de acesso
</commit_message>
<xml_diff>
--- a/db/sod_database.xlsx
+++ b/db/sod_database.xlsx
@@ -613,7 +613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -662,6 +662,28 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sia-estacio</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>professor</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sia-estacio</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>aluno</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
validacao save modal usuarios
</commit_message>
<xml_diff>
--- a/db/sod_database.xlsx
+++ b/db/sod_database.xlsx
@@ -754,7 +754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,7 +781,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>12345678901</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -795,8 +795,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>12345678901</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -805,82 +807,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>aluno</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>12345678901</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>sava</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>aluno</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>131313</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>sava</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4324234</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>financeiro</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>131313</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>sava</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>12345678901</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>sava</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>aluno</t>
+          <t>professor</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
validacao matriz na criacao de usuarios
</commit_message>
<xml_diff>
--- a/db/sod_database.xlsx
+++ b/db/sod_database.xlsx
@@ -543,7 +543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,57 @@
         </is>
       </c>
       <c r="C5" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sava</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>tecnico</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>novo_sistema</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>novo_perfil</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>teste</t>
         </is>
@@ -647,7 +698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,50 +747,6 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>professor</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>sia-estacio</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>professor</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>sia-estacio</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>aluno</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>financeiro</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>funcionário</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>sava</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>aluno</t>
         </is>
       </c>
     </row>
@@ -754,7 +761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,22 +797,37 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sava</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>aluno</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>sava</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>professor</t>
         </is>

</xml_diff>